<commit_message>
Switch to using expect to change; fix batch-ingest test to test intended behavior
</commit_message>
<xml_diff>
--- a/spec/fixtures/batch_manifest_derivatives.xlsx
+++ b/spec/fixtures/batch_manifest_derivatives.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -38,6 +38,9 @@
     <t>File</t>
   </si>
   <si>
+    <t>Skip transcoding</t>
+  </si>
+  <si>
     <t>Offset</t>
   </si>
   <si>
@@ -53,7 +56,10 @@
     <t>Ut minus ut accusantium odio autem odit.</t>
   </si>
   <si>
-    <t>videoshort.mp4</t>
+    <t>derivative.mp4</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -61,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -103,7 +109,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -112,51 +118,51 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -166,34 +172,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1906976744186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1953488372093"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5116279069767"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3906976744186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.2279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.0093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5116279069767"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5116279069767"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -215,33 +222,39 @@
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="frances.dickens@reichel.com"/>
+    <hyperlink display="frances.dickens@reichel.com" ref="B1" r:id="rId1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Use existing derivative fixtures
</commit_message>
<xml_diff>
--- a/spec/fixtures/batch_manifest_derivatives.xlsx
+++ b/spec/fixtures/batch_manifest_derivatives.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
     <t>Ut minus ut accusantium odio autem odit.</t>
   </si>
   <si>
-    <t>derivative.mp4</t>
+    <t>videoshort.mp4</t>
   </si>
   <si>
     <t>yes</t>
@@ -67,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -109,7 +109,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -118,51 +118,51 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -170,28 +170,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5116279069767"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.2279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0093023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5116279069767"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.2296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5111111111111"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -200,7 +201,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -226,7 +227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -250,11 +251,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="frances.dickens@reichel.com" ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" display="frances.dickens@reichel.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>